<commit_message>
Chnages in user interface
</commit_message>
<xml_diff>
--- a/backend/Controllers/public/student_data.xlsx
+++ b/backend/Controllers/public/student_data.xlsx
@@ -397,13 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>